<commit_message>
bijna alle vragen van de taak 50% zijn ingevuld
</commit_message>
<xml_diff>
--- a/school/50%.xlsx
+++ b/school/50%.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debakkers\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ptibe-my.sharepoint.com/personal/stan_debakker_leerling_pti_be/Documents/programeren/Arduino/6TWEA/grap-6TWEA/school/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0BF384-C0C2-4E7B-A4A5-42184FE68E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{DB0BF384-C0C2-4E7B-A4A5-42184FE68E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AB7F1DC-0B7A-47B8-8250-D59BBCC4B2CE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8D02C5D0-9212-4D29-AED6-60E55B7BB112}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">voldoende </t>
   </si>
@@ -83,12 +83,6 @@
     <t xml:space="preserve">Werkt er 50%? </t>
   </si>
   <si>
-    <t>er word soms "gezeeverd" (over ander zaken gepraad)</t>
-  </si>
-  <si>
-    <t>soms praat ik mee</t>
-  </si>
-  <si>
     <t>ik heb de robot van in het begin gekregen en de eerste niet goed werkende versie van de ESP32 addon is er al</t>
   </si>
   <si>
@@ -99,6 +93,18 @@
   </si>
   <si>
     <t>ja want ik heb tijdens studie 1 alle code om de robot te besturen gemaakt er moet allen nog maar eenbeetje code worden geschreven voor de zaken die ik toevoeg die ik theoretisch al heb gemaakt</t>
+  </si>
+  <si>
+    <t>als ik het met draatjes verbind wat minder mooi is werkt het</t>
+  </si>
+  <si>
+    <t>er word soms "gezeeverd" (over ander zaken gepraad) maar ik werk wel veel thuis</t>
+  </si>
+  <si>
+    <t>soms praat ik mee maar ik werk wel veel thuis</t>
+  </si>
+  <si>
+    <t>ik weet hoe ik de problemen die ik nu heb ga oplossen want ik heb all veel tetorials gevold</t>
   </si>
 </sst>
 </file>
@@ -676,6 +682,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -998,7 +1008,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1037,7 +1047,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="6"/>
       <c r="E2" s="8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F2" s="10"/>
     </row>
@@ -1049,7 +1059,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="6"/>
       <c r="E3" s="8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F3" s="10"/>
     </row>
@@ -1073,7 +1083,9 @@
       <c r="C5" s="4"/>
       <c r="D5" s="6"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
@@ -1084,7 +1096,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="8"/>
       <c r="F6" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1096,7 +1108,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="8"/>
       <c r="F7" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1107,7 +1119,9 @@
       <c r="C8" s="12"/>
       <c r="D8" s="6"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
@@ -1115,7 +1129,7 @@
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -1127,7 +1141,7 @@
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -1168,20 +1182,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="a0473d4f-1cca-4074-b684-28dae071d4ec" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="a0473d4f-1cca-4074-b684-28dae071d4ec" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1335,19 +1349,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731A669D-56AC-4B51-8DC7-52EAB750F91F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C191BD4F-77EE-490B-8F19-92852807F23F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a0473d4f-1cca-4074-b684-28dae071d4ec"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731A669D-56AC-4B51-8DC7-52EAB750F91F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
wek '50%' voledig af
</commit_message>
<xml_diff>
--- a/school/50%.xlsx
+++ b/school/50%.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ptibe-my.sharepoint.com/personal/stan_debakker_leerling_pti_be/Documents/programeren/Arduino/6TWEA/grap-6TWEA/school/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debakkers\OneDrive - PTI-Kortrijk\programeren\Arduino\6TWEA\grap-6TWEA\school\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{DB0BF384-C0C2-4E7B-A4A5-42184FE68E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AB7F1DC-0B7A-47B8-8250-D59BBCC4B2CE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DF46AB-E7DC-481D-BB26-773918D3DABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8D02C5D0-9212-4D29-AED6-60E55B7BB112}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">voldoende </t>
   </si>
@@ -89,9 +89,6 @@
     <t>de addon PCB</t>
   </si>
   <si>
-    <t>alles wat ik wiel upgraden</t>
-  </si>
-  <si>
     <t>ja want ik heb tijdens studie 1 alle code om de robot te besturen gemaakt er moet allen nog maar eenbeetje code worden geschreven voor de zaken die ik toevoeg die ik theoretisch al heb gemaakt</t>
   </si>
   <si>
@@ -105,6 +102,12 @@
   </si>
   <si>
     <t>ik weet hoe ik de problemen die ik nu heb ga oplossen want ik heb all veel tetorials gevold</t>
+  </si>
+  <si>
+    <t>ik weet hoe ik het hooft en de lijnsensoren wil verbeteren bij het hoofdbord zal ik allen nog de buck/boost covertor onderdelen opzoeken</t>
+  </si>
+  <si>
+    <t>alles wat ik wil upgraden</t>
   </si>
 </sst>
 </file>
@@ -682,10 +685,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1007,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C96AB71-7ADD-4701-BB67-7C0003342D1F}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1047,7 +1046,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="6"/>
       <c r="E2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="10"/>
     </row>
@@ -1059,7 +1058,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="6"/>
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="10"/>
     </row>
@@ -1073,7 +1072,9 @@
       <c r="C4" s="4"/>
       <c r="D4" s="6"/>
       <c r="E4" s="8"/>
-      <c r="F4" s="10"/>
+      <c r="F4" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
@@ -1084,7 +1085,7 @@
       <c r="D5" s="6"/>
       <c r="E5" s="8"/>
       <c r="F5" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
@@ -1096,7 +1097,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="8"/>
       <c r="F6" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="47.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1120,7 +1121,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="8"/>
       <c r="F8" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.35">
@@ -1141,7 +1142,7 @@
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -1182,20 +1183,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="a0473d4f-1cca-4074-b684-28dae071d4ec" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="a0473d4f-1cca-4074-b684-28dae071d4ec" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1349,19 +1350,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731A669D-56AC-4B51-8DC7-52EAB750F91F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C191BD4F-77EE-490B-8F19-92852807F23F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a0473d4f-1cca-4074-b684-28dae071d4ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C191BD4F-77EE-490B-8F19-92852807F23F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731A669D-56AC-4B51-8DC7-52EAB750F91F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a0473d4f-1cca-4074-b684-28dae071d4ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>